<commit_message>
Add H-Score to smoke test
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/Results.xlsx
+++ b/tests/testthat/test_data/Results.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Cell Percents" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Cell Densities" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Mean Expression" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="H-Score" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Slide Summary'!$1:$1</definedName>
@@ -18,12 +19,13 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Cell Percents'!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Cell Densities'!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Mean Expression'!$1:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'H-Score'!$1:$3</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">Slide ID</t>
   </si>
@@ -89,13 +91,37 @@
   </si>
   <si>
     <t xml:space="preserve">CK+ Membrane PDL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-Score, Membrane PDL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cells per Bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of Total Cells per Bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-Score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="50">
+  <numFmts count="58">
     <numFmt numFmtId="50000" formatCode="0%"/>
     <numFmt numFmtId="50001" formatCode="0%"/>
     <numFmt numFmtId="50002" formatCode="0%"/>
@@ -146,6 +172,14 @@
     <numFmt numFmtId="50047" formatCode="0.00"/>
     <numFmt numFmtId="50048" formatCode="0.00"/>
     <numFmt numFmtId="50049" formatCode="0.00"/>
+    <numFmt numFmtId="50050" formatCode="0.0%"/>
+    <numFmt numFmtId="50051" formatCode="0.0%"/>
+    <numFmt numFmtId="50052" formatCode="0.0%"/>
+    <numFmt numFmtId="50053" formatCode="0.0%"/>
+    <numFmt numFmtId="50054" formatCode="0.0%"/>
+    <numFmt numFmtId="50055" formatCode="0.0%"/>
+    <numFmt numFmtId="50056" formatCode="0.0%"/>
+    <numFmt numFmtId="50057" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -175,7 +209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -301,11 +335,19 @@
         <color rgb="FF000000"/>
       </top>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -385,6 +427,30 @@
     <xf numFmtId="50047" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="50048" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="50049" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="50050" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="50051" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="50052" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="50053" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="50054" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="50055" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="50056" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="50057" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1714,4 +1780,418 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" scale="100" fitToWidth="0" fitToHeight="0" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="11.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="11.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="72" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="76" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="16" t="n">
+        <v>534</v>
+      </c>
+      <c r="D4" s="18" t="n">
+        <v>189</v>
+      </c>
+      <c r="E4" s="18" t="n">
+        <v>91</v>
+      </c>
+      <c r="F4" s="18" t="n">
+        <v>83</v>
+      </c>
+      <c r="G4" s="77" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="H4" s="77" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="I4" s="77" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="J4" s="77" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="K4" s="17" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>104</v>
+      </c>
+      <c r="D5" t="n">
+        <v>175</v>
+      </c>
+      <c r="E5" t="n">
+        <v>287</v>
+      </c>
+      <c r="F5" t="n">
+        <v>269</v>
+      </c>
+      <c r="G5" s="80" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="H5" s="80" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="I5" s="80" t="n">
+        <v>0.344</v>
+      </c>
+      <c r="J5" s="80" t="n">
+        <v>0.322</v>
+      </c>
+      <c r="K5" s="10" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>638</v>
+      </c>
+      <c r="D6" t="n">
+        <v>364</v>
+      </c>
+      <c r="E6" t="n">
+        <v>378</v>
+      </c>
+      <c r="F6" t="n">
+        <v>352</v>
+      </c>
+      <c r="G6" s="80" t="n">
+        <v>0.368</v>
+      </c>
+      <c r="H6" s="80" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="I6" s="80" t="n">
+        <v>0.218</v>
+      </c>
+      <c r="J6" s="80" t="n">
+        <v>0.203</v>
+      </c>
+      <c r="K6" s="10" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="16" t="n">
+        <v>36</v>
+      </c>
+      <c r="D7" s="18" t="n">
+        <v>219</v>
+      </c>
+      <c r="E7" s="18" t="n">
+        <v>159</v>
+      </c>
+      <c r="F7" s="18" t="n">
+        <v>220</v>
+      </c>
+      <c r="G7" s="78" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="H7" s="78" t="n">
+        <v>0.345</v>
+      </c>
+      <c r="I7" s="78" t="n">
+        <v>0.251</v>
+      </c>
+      <c r="J7" s="78" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="K7" s="17" t="n">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>109</v>
+      </c>
+      <c r="D8" t="n">
+        <v>313</v>
+      </c>
+      <c r="E8" t="n">
+        <v>421</v>
+      </c>
+      <c r="F8" t="n">
+        <v>437</v>
+      </c>
+      <c r="G8" s="80" t="n">
+        <v>0.085</v>
+      </c>
+      <c r="H8" s="80" t="n">
+        <v>0.245</v>
+      </c>
+      <c r="I8" s="80" t="n">
+        <v>0.329</v>
+      </c>
+      <c r="J8" s="80" t="n">
+        <v>0.341</v>
+      </c>
+      <c r="K8" s="10" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="9" t="n">
+        <v>145</v>
+      </c>
+      <c r="D9" t="n">
+        <v>532</v>
+      </c>
+      <c r="E9" t="n">
+        <v>580</v>
+      </c>
+      <c r="F9" t="n">
+        <v>657</v>
+      </c>
+      <c r="G9" s="80" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="H9" s="80" t="n">
+        <v>0.278</v>
+      </c>
+      <c r="I9" s="80" t="n">
+        <v>0.303</v>
+      </c>
+      <c r="J9" s="80" t="n">
+        <v>0.343</v>
+      </c>
+      <c r="K9" s="10" t="n">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="16" t="n">
+        <v>199</v>
+      </c>
+      <c r="D10" s="18" t="n">
+        <v>192</v>
+      </c>
+      <c r="E10" s="18" t="n">
+        <v>136</v>
+      </c>
+      <c r="F10" s="18" t="n">
+        <v>80</v>
+      </c>
+      <c r="G10" s="79" t="n">
+        <v>0.328</v>
+      </c>
+      <c r="H10" s="79" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="I10" s="79" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="J10" s="79" t="n">
+        <v>0.132</v>
+      </c>
+      <c r="K10" s="17" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9" t="n">
+        <v>382</v>
+      </c>
+      <c r="D11" t="n">
+        <v>275</v>
+      </c>
+      <c r="E11" t="n">
+        <v>270</v>
+      </c>
+      <c r="F11" t="n">
+        <v>275</v>
+      </c>
+      <c r="G11" s="80" t="n">
+        <v>0.318</v>
+      </c>
+      <c r="H11" s="80" t="n">
+        <v>0.229</v>
+      </c>
+      <c r="I11" s="80" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="J11" s="80" t="n">
+        <v>0.229</v>
+      </c>
+      <c r="K11" s="10" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="12" t="n">
+        <v>581</v>
+      </c>
+      <c r="D12" s="14" t="n">
+        <v>467</v>
+      </c>
+      <c r="E12" s="14" t="n">
+        <v>406</v>
+      </c>
+      <c r="F12" s="14" t="n">
+        <v>355</v>
+      </c>
+      <c r="G12" s="14" t="n">
+        <v>0.321</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <v>0.258</v>
+      </c>
+      <c r="I12" s="14" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="J12" s="14" t="n">
+        <v>0.196</v>
+      </c>
+      <c r="K12" s="13" t="n">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="K2:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" scale="100" fitToWidth="0" fitToHeight="0" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add test for multiple markers per phenotype. Fix chart titles when there are multiple expression charts.
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/Results.xlsx
+++ b/tests/testthat/test_data/Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">Slide ID</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t xml:space="preserve">CD8+ Membrane PDL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD8+ Membrane PD1</t>
   </si>
   <si>
     <t xml:space="preserve">CD68+ Membrane PDL1</t>
@@ -1637,6 +1640,7 @@
     <col min="3" max="3" width="14.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="14.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="14.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="14.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1650,7 +1654,8 @@
         <v>18</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="E1" s="5"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
@@ -1668,6 +1673,9 @@
       <c r="E2" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="F2" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="15" t="s">
@@ -1680,9 +1688,12 @@
         <v>0.856125</v>
       </c>
       <c r="D3" s="61" t="n">
+        <v>7.434</v>
+      </c>
+      <c r="E3" s="61" t="n">
         <v>5.96084615384615</v>
       </c>
-      <c r="E3" s="60" t="n">
+      <c r="F3" s="60" t="n">
         <v>0.947405307599517</v>
       </c>
     </row>
@@ -1697,9 +1708,12 @@
         <v>2.03454545454545</v>
       </c>
       <c r="D4" s="68" t="n">
+        <v>6.93463636363636</v>
+      </c>
+      <c r="E4" s="68" t="n">
         <v>5.03644186046512</v>
       </c>
-      <c r="E4" s="55" t="n">
+      <c r="F4" s="55" t="n">
         <v>2.0013</v>
       </c>
     </row>
@@ -1714,9 +1728,12 @@
         <v>3.3575</v>
       </c>
       <c r="D5" s="64" t="n">
+        <v>2.85891666666667</v>
+      </c>
+      <c r="E5" s="64" t="n">
         <v>8.04607407407407</v>
       </c>
-      <c r="E5" s="63" t="n">
+      <c r="F5" s="63" t="n">
         <v>3.70934630350195</v>
       </c>
     </row>
@@ -1731,9 +1748,12 @@
         <v>2.33060714285714</v>
       </c>
       <c r="D6" s="68" t="n">
+        <v>3.91146428571429</v>
+      </c>
+      <c r="E6" s="68" t="n">
         <v>6.45196590909091</v>
       </c>
-      <c r="E6" s="55" t="n">
+      <c r="F6" s="55" t="n">
         <v>3.55710714285714</v>
       </c>
     </row>
@@ -1748,9 +1768,12 @@
         <v>1.94514285714286</v>
       </c>
       <c r="D7" s="67" t="n">
+        <v>5.64085714285714</v>
+      </c>
+      <c r="E7" s="67" t="n">
         <v>4.96588888888889</v>
       </c>
-      <c r="E7" s="66" t="n">
+      <c r="F7" s="66" t="n">
         <v>1.50520488721805</v>
       </c>
     </row>
@@ -1765,15 +1788,18 @@
         <v>1.48879069767442</v>
       </c>
       <c r="D8" s="58" t="n">
+        <v>5.65262790697674</v>
+      </c>
+      <c r="E8" s="58" t="n">
         <v>5.38612962962963</v>
       </c>
-      <c r="E8" s="57" t="n">
+      <c r="F8" s="57" t="n">
         <v>2.77561538461538</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C1:F1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
@@ -1802,7 +1828,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -1817,19 +1843,19 @@
       <c r="A2" s="71"/>
       <c r="B2" s="71"/>
       <c r="C2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="69"/>
       <c r="E2" s="69"/>
       <c r="F2" s="70"/>
       <c r="G2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
       <c r="J2" s="70"/>
       <c r="K2" s="72" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -1840,31 +1866,31 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="H3" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="I3" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="75" t="s">
-        <v>27</v>
-      </c>
       <c r="J3" s="76" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Fix Results.xlsx to match modified H-Score thresholds. Comment out some dev code that should not be checked in .
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/Results.xlsx
+++ b/tests/testthat/test_data/Results.xlsx
@@ -1901,31 +1901,31 @@
         <v>12</v>
       </c>
       <c r="C4" s="16" t="n">
-        <v>534</v>
+        <v>814</v>
       </c>
       <c r="D4" s="18" t="n">
-        <v>189</v>
+        <v>56</v>
       </c>
       <c r="E4" s="18" t="n">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="G4" s="77" t="n">
-        <v>0.595</v>
+        <v>0.907</v>
       </c>
       <c r="H4" s="77" t="n">
-        <v>0.211</v>
+        <v>0.062</v>
       </c>
       <c r="I4" s="77" t="n">
-        <v>0.101</v>
+        <v>0.02</v>
       </c>
       <c r="J4" s="77" t="n">
-        <v>0.093</v>
+        <v>0.01</v>
       </c>
       <c r="K4" s="17" t="n">
-        <v>69</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -1936,31 +1936,31 @@
         <v>13</v>
       </c>
       <c r="C5" s="9" t="n">
-        <v>104</v>
+        <v>566</v>
       </c>
       <c r="D5" t="n">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E5" t="n">
-        <v>287</v>
+        <v>51</v>
       </c>
       <c r="F5" t="n">
-        <v>269</v>
+        <v>49</v>
       </c>
       <c r="G5" s="80" t="n">
-        <v>0.125</v>
+        <v>0.678</v>
       </c>
       <c r="H5" s="80" t="n">
-        <v>0.21</v>
+        <v>0.202</v>
       </c>
       <c r="I5" s="80" t="n">
-        <v>0.344</v>
+        <v>0.061</v>
       </c>
       <c r="J5" s="80" t="n">
-        <v>0.322</v>
+        <v>0.059</v>
       </c>
       <c r="K5" s="10" t="n">
-        <v>186</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -1971,31 +1971,31 @@
         <v>14</v>
       </c>
       <c r="C6" s="9" t="n">
-        <v>638</v>
+        <v>1380</v>
       </c>
       <c r="D6" t="n">
-        <v>364</v>
+        <v>225</v>
       </c>
       <c r="E6" t="n">
-        <v>378</v>
+        <v>69</v>
       </c>
       <c r="F6" t="n">
-        <v>352</v>
+        <v>58</v>
       </c>
       <c r="G6" s="80" t="n">
-        <v>0.368</v>
+        <v>0.797</v>
       </c>
       <c r="H6" s="80" t="n">
-        <v>0.21</v>
+        <v>0.13</v>
       </c>
       <c r="I6" s="80" t="n">
-        <v>0.218</v>
+        <v>0.04</v>
       </c>
       <c r="J6" s="80" t="n">
-        <v>0.203</v>
+        <v>0.033</v>
       </c>
       <c r="K6" s="10" t="n">
-        <v>125</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
@@ -2006,31 +2006,31 @@
         <v>12</v>
       </c>
       <c r="C7" s="16" t="n">
-        <v>36</v>
+        <v>414</v>
       </c>
       <c r="D7" s="18" t="n">
-        <v>219</v>
+        <v>109</v>
       </c>
       <c r="E7" s="18" t="n">
-        <v>159</v>
+        <v>56</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>220</v>
+        <v>55</v>
       </c>
       <c r="G7" s="78" t="n">
-        <v>0.057</v>
+        <v>0.653</v>
       </c>
       <c r="H7" s="78" t="n">
-        <v>0.345</v>
+        <v>0.172</v>
       </c>
       <c r="I7" s="78" t="n">
-        <v>0.251</v>
+        <v>0.088</v>
       </c>
       <c r="J7" s="78" t="n">
-        <v>0.347</v>
+        <v>0.087</v>
       </c>
       <c r="K7" s="17" t="n">
-        <v>189</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
@@ -2041,31 +2041,31 @@
         <v>13</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>109</v>
+        <v>843</v>
       </c>
       <c r="D8" t="n">
-        <v>313</v>
+        <v>263</v>
       </c>
       <c r="E8" t="n">
-        <v>421</v>
+        <v>72</v>
       </c>
       <c r="F8" t="n">
-        <v>437</v>
+        <v>102</v>
       </c>
       <c r="G8" s="80" t="n">
-        <v>0.085</v>
+        <v>0.659</v>
       </c>
       <c r="H8" s="80" t="n">
-        <v>0.245</v>
+        <v>0.205</v>
       </c>
       <c r="I8" s="80" t="n">
-        <v>0.329</v>
+        <v>0.056</v>
       </c>
       <c r="J8" s="80" t="n">
-        <v>0.341</v>
+        <v>0.08</v>
       </c>
       <c r="K8" s="10" t="n">
-        <v>193</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
@@ -2076,31 +2076,31 @@
         <v>14</v>
       </c>
       <c r="C9" s="9" t="n">
-        <v>145</v>
+        <v>1257</v>
       </c>
       <c r="D9" t="n">
-        <v>532</v>
+        <v>372</v>
       </c>
       <c r="E9" t="n">
-        <v>580</v>
+        <v>128</v>
       </c>
       <c r="F9" t="n">
-        <v>657</v>
+        <v>157</v>
       </c>
       <c r="G9" s="80" t="n">
-        <v>0.076</v>
+        <v>0.657</v>
       </c>
       <c r="H9" s="80" t="n">
-        <v>0.278</v>
+        <v>0.194</v>
       </c>
       <c r="I9" s="80" t="n">
-        <v>0.303</v>
+        <v>0.067</v>
       </c>
       <c r="J9" s="80" t="n">
-        <v>0.343</v>
+        <v>0.082</v>
       </c>
       <c r="K9" s="10" t="n">
-        <v>191</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10">
@@ -2111,31 +2111,31 @@
         <v>12</v>
       </c>
       <c r="C10" s="16" t="n">
-        <v>199</v>
+        <v>527</v>
       </c>
       <c r="D10" s="18" t="n">
-        <v>192</v>
+        <v>57</v>
       </c>
       <c r="E10" s="18" t="n">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="G10" s="79" t="n">
-        <v>0.328</v>
+        <v>0.868</v>
       </c>
       <c r="H10" s="79" t="n">
-        <v>0.316</v>
+        <v>0.094</v>
       </c>
       <c r="I10" s="79" t="n">
-        <v>0.224</v>
+        <v>0.016</v>
       </c>
       <c r="J10" s="79" t="n">
-        <v>0.132</v>
+        <v>0.021</v>
       </c>
       <c r="K10" s="17" t="n">
-        <v>116</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
@@ -2146,31 +2146,31 @@
         <v>13</v>
       </c>
       <c r="C11" s="9" t="n">
-        <v>382</v>
+        <v>927</v>
       </c>
       <c r="D11" t="n">
-        <v>275</v>
+        <v>164</v>
       </c>
       <c r="E11" t="n">
-        <v>270</v>
+        <v>66</v>
       </c>
       <c r="F11" t="n">
-        <v>275</v>
+        <v>45</v>
       </c>
       <c r="G11" s="80" t="n">
-        <v>0.318</v>
+        <v>0.771</v>
       </c>
       <c r="H11" s="80" t="n">
-        <v>0.229</v>
+        <v>0.136</v>
       </c>
       <c r="I11" s="80" t="n">
-        <v>0.225</v>
+        <v>0.055</v>
       </c>
       <c r="J11" s="80" t="n">
-        <v>0.229</v>
+        <v>0.037</v>
       </c>
       <c r="K11" s="10" t="n">
-        <v>137</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
@@ -2181,31 +2181,31 @@
         <v>14</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>581</v>
+        <v>1454</v>
       </c>
       <c r="D12" s="14" t="n">
-        <v>467</v>
+        <v>221</v>
       </c>
       <c r="E12" s="14" t="n">
-        <v>406</v>
+        <v>76</v>
       </c>
       <c r="F12" s="14" t="n">
-        <v>355</v>
+        <v>58</v>
       </c>
       <c r="G12" s="14" t="n">
-        <v>0.321</v>
+        <v>0.804</v>
       </c>
       <c r="H12" s="14" t="n">
-        <v>0.258</v>
+        <v>0.122</v>
       </c>
       <c r="I12" s="14" t="n">
-        <v>0.224</v>
+        <v>0.042</v>
       </c>
       <c r="J12" s="14" t="n">
-        <v>0.196</v>
+        <v>0.032</v>
       </c>
       <c r="K12" s="13" t="n">
-        <v>129</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabs with H-Score results include the scored marker name, in support of #49
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/Results.xlsx
+++ b/tests/testthat/test_data/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\phenoptrReports\tests\testthat\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\phenoptrReports\tests\testthat\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFD35CA-5E4F-411F-AB6B-035C79537070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF79ED4-BE91-4F58-9FD4-860E1C3DA214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12384" yWindow="1668" windowWidth="13512" windowHeight="12252" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14160" yWindow="2016" windowWidth="13512" windowHeight="12252" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slide Summary" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Cell Percents" sheetId="3" r:id="rId3"/>
     <sheet name="Cell Densities" sheetId="4" r:id="rId4"/>
     <sheet name="Mean Expression" sheetId="5" r:id="rId5"/>
-    <sheet name="H-Score" sheetId="6" r:id="rId6"/>
-    <sheet name="H-Score CD8+" sheetId="7" r:id="rId7"/>
-    <sheet name="H-Score CK+_Membrane PDL1 (Opal" sheetId="8" r:id="rId8"/>
+    <sheet name="H-Score, PDL1" sheetId="6" r:id="rId6"/>
+    <sheet name="H-Score, PDL1, CD8+" sheetId="7" r:id="rId7"/>
+    <sheet name="H-Score, PDL1, CK+_PDL1&gt;1" sheetId="8" r:id="rId8"/>
     <sheet name="Nearest Neighbors" sheetId="9" r:id="rId9"/>
     <sheet name="Count Within" sheetId="10" r:id="rId10"/>
   </sheets>
@@ -29,9 +29,9 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Cell Densities'!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Cell Percents'!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="9">'Count Within'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="5">'H-Score'!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'H-Score CD8+'!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">'H-Score CK+_Membrane PDL1 (Opal'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'H-Score, PDL1'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">'H-Score, PDL1, CD8+'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">'H-Score, PDL1, CK+_PDL1&gt;1'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Mean Expression'!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">'Nearest Neighbors'!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Slide Summary'!$1:$1</definedName>
@@ -20641,7 +20641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -20911,7 +20911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -21324,7 +21326,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -21737,7 +21741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -22150,7 +22156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I326"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>